<commit_message>
addming intreg.py and intreg.xlsx
</commit_message>
<xml_diff>
--- a/BOND_EQT/intreg.xlsx
+++ b/BOND_EQT/intreg.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c060ac0a7f9c7ae2/main/CRAMC_Desktop/EU/BOND_EQT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c060ac0a7f9c7ae2/main/DELL_NB/EU/BOND_EQT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="11_F25DC773A252ABDACC10481FB9187D7A5BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09A88472-87F7-4826-9AE3-5188F2278D61}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="11_F25DC773A252ABDACC10481FB9187D7A5BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FED15DE4-2C26-46D7-A714-B42A0555DF4B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="480" windowWidth="21840" windowHeight="38040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>阿里巴巴集团控股有限公司</t>
   </si>
@@ -69,9 +69,6 @@
     <t>唯品会控股有限公司</t>
   </si>
   <si>
-    <t>拼多多</t>
-  </si>
-  <si>
     <t>网易股份有限公司</t>
   </si>
   <si>
@@ -139,6 +136,12 @@
   </si>
   <si>
     <t>市值</t>
+  </si>
+  <si>
+    <t>腾讯控股有限公司</t>
+  </si>
+  <si>
+    <t>Tencent Holdings Ltd</t>
   </si>
 </sst>
 </file>
@@ -147,8 +150,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -200,10 +203,9 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -212,10 +214,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -233,131 +235,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
-<volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <volType type="realTimeData">
-    <main first="bofaddin.rtdserver">
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDP|10451871569717875365</stp>
-        <tr r="F15" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDP|12432712876131454902</stp>
-        <tr r="F17" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDP|16082249521485208816</stp>
-        <tr r="F20" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDP|11816260256696852838</stp>
-        <tr r="F12" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDP|12500996684167741970</stp>
-        <tr r="F9" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDP|16043548645853954675</stp>
-        <tr r="F11" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDP|11099255637106709663</stp>
-        <tr r="F6" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDP|12298139085475513867</stp>
-        <tr r="F16" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDP|14425486046770704120</stp>
-        <tr r="F8" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDP|12622201445880920143</stp>
-        <tr r="F18" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDP|13874129373940932050</stp>
-        <tr r="F5" s="1"/>
-      </tp>
-    </main>
-    <main first="bofaddin.rtdserver">
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDP|2276936849975299420</stp>
-        <tr r="F14" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDP|6217847001135281524</stp>
-        <tr r="F2" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDP|9421402977173882382</stp>
-        <tr r="F13" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDP|5769056425601775234</stp>
-        <tr r="F7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDP|2621969287410080617</stp>
-        <tr r="F10" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDP|5656936180027779467</stp>
-        <tr r="F3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDP|2666215638020682224</stp>
-        <tr r="F19" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDP|2061247741526120363</stp>
-        <tr r="F4" s="1"/>
-      </tp>
-    </main>
-  </volType>
-</volTypes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -626,452 +503,468 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="27.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="str" cm="1">
+      <c r="B2" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="B2" ca="1">_xll.BDP($B2,B$2)</f>
         <v>Alibaba Group Holding Ltd</v>
       </c>
-      <c r="C2" s="1">
-        <v>2.3080225676250881</v>
-      </c>
-      <c r="D2" s="2">
-        <v>5.3163868751910703E-2</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="10" cm="1">
-        <f t="array" aca="1" ref="F2" ca="1">_xll.BDP($B2,F$4,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
+      <c r="C2" s="9" cm="1">
+        <f t="array" aca="1" ref="C2" ca="1">_xll.BDP($B2,C$5,C$4,C$2)</f>
+        <v>2.0860661873116659</v>
+      </c>
+      <c r="D2" s="1">
+        <v>6.8094577815983826E-2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="8" cm="1">
+        <f t="array" aca="1" ref="F2" ca="1">_xll.BDP($B2,F$5,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
         <v>330.30706301880008</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="9">
+        <v>5.6622793655752259</v>
+      </c>
+      <c r="D3" s="1">
+        <v>8.3052589275886879E-2</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="8">
+        <v>604.88031043562341</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="B3" ca="1">_xll.BDP($B3,B$2)</f>
+      <c r="B4" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="B4" ca="1">_xll.BDP($B4,B$2)</f>
         <v>JD.com Inc</v>
       </c>
-      <c r="C3" s="1">
-        <v>0.38187992539540094</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C4" s="9" cm="1">
+        <f t="array" aca="1" ref="C4" ca="1">_xll.BDP($B4,C$5,C$4,C$2)</f>
+        <v>0.34399322055315984</v>
+      </c>
+      <c r="D4" s="1">
         <v>6.2537487280635018E-2</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="10" cm="1">
-        <f t="array" aca="1" ref="F3" ca="1">_xll.BDP($B3,F$4,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
+      <c r="E4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8" cm="1">
+        <f t="array" aca="1" ref="F4" ca="1">_xll.BDP($B4,F$5,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
         <v>66.02246996400001</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="B4" ca="1">_xll.BDP($B4,B$2)</f>
+      <c r="B5" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="B5" ca="1">_xll.BDP($B5,B$2)</f>
         <v>Vipshop Holdings Ltd</v>
       </c>
-      <c r="C4" s="1">
-        <v>0.5658458867488203</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C5" s="9" cm="1">
+        <f t="array" aca="1" ref="C5" ca="1">_xll.BDP($B5,C$5,C$4,C$2)</f>
+        <v>0.54318877026029688</v>
+      </c>
+      <c r="D5" s="1">
         <v>1.3084924495458727E-2</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="10" cm="1">
-        <f t="array" aca="1" ref="F4" ca="1">_xll.BDP($B4,F$4,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
+      <c r="E5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="8" cm="1">
+        <f t="array" aca="1" ref="F5" ca="1">_xll.BDP($B5,F$5,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
         <v>8.454629270782533</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="str" cm="1">
-        <f t="array" aca="1" ref="B5" ca="1">_xll.BDP($B5,B$2)</f>
-        <v>PDD Holdings Inc</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2.5271306475526276</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0.16802059151292981</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="10" cm="1">
-        <f t="array" aca="1" ref="F5" ca="1">_xll.BDP($B5,F$4,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
-        <v>163.8471571577</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="str" cm="1">
+      <c r="B6" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="B6" ca="1">_xll.BDP($B6,B$2)</f>
         <v>NetEase Inc</v>
       </c>
-      <c r="C6" s="1">
-        <v>4.2753219925367798</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6" s="9" cm="1">
+        <f t="array" aca="1" ref="C6" ca="1">_xll.BDP($B6,C$5,C$4,C$2)</f>
+        <v>3.7477457722184231</v>
+      </c>
+      <c r="D6" s="1">
         <v>7.3197360000651912E-2</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="10" cm="1">
-        <f t="array" aca="1" ref="F6" ca="1">_xll.BDP($B6,F$4,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
+      <c r="E6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8" cm="1">
+        <f t="array" aca="1" ref="F6" ca="1">_xll.BDP($B6,F$5,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
         <v>67.345894418459991</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="5" t="str" cm="1">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="B7" ca="1">_xll.BDP($B7,B$2)</f>
         <v>Kanzhun Ltd</v>
       </c>
-      <c r="C7" s="1">
-        <v>7.227477251636075</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.12796719096613285</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="10" cm="1">
-        <f t="array" aca="1" ref="F7" ca="1">_xll.BDP($B7,F$4,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
+      <c r="C7" s="9" cm="1">
+        <f t="array" aca="1" ref="C7" ca="1">_xll.BDP($B7,C$5,C$4,C$2)</f>
+        <v>5.6698050644122526</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.21116737799381169</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8" cm="1">
+        <f t="array" aca="1" ref="F7" ca="1">_xll.BDP($B7,F$5,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
         <v>8.2782603681749993</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="5" t="str" cm="1">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="B8" ca="1">_xll.BDP($B8,B$2)</f>
         <v>Kuaishou Technology</v>
       </c>
-      <c r="C8" s="1">
-        <v>1.902224443937613</v>
-      </c>
-      <c r="D8" s="2">
-        <v>7.4507284311895239E-2</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="10" cm="1">
-        <f t="array" aca="1" ref="F8" ca="1">_xll.BDP($B8,F$4,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
+      <c r="C8" s="9" cm="1">
+        <f t="array" aca="1" ref="C8" ca="1">_xll.BDP($B8,C$5,C$4,C$2)</f>
+        <v>1.7163878124689402</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.10699019368214446</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="8" cm="1">
+        <f t="array" aca="1" ref="F8" ca="1">_xll.BDP($B8,F$5,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
         <v>283.38758371454998</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="5" t="str" cm="1">
+      <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="B9" ca="1">_xll.BDP($B9,B$2)</f>
         <v>Bilibili Inc</v>
       </c>
-      <c r="C9" s="1">
-        <v>2.2809970927800145</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="C9" s="9" cm="1">
+        <f t="array" aca="1" ref="C9" ca="1">_xll.BDP($B9,C$5,C$4,C$2)</f>
+        <v>1.9207377294580785</v>
+      </c>
+      <c r="D9" s="1">
         <v>0.10467857952675708</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="10" cm="1">
-        <f t="array" aca="1" ref="F9" ca="1">_xll.BDP($B9,F$4,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
+      <c r="E9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="8" cm="1">
+        <f t="array" aca="1" ref="F9" ca="1">_xll.BDP($B9,F$5,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
         <v>9.5921224650899983</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="5" t="str" cm="1">
+      <c r="A10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="B10" ca="1">_xll.BDP($B10,B$2)</f>
         <v>Baidu Inc</v>
       </c>
-      <c r="C10" s="1">
-        <v>1.7491987691546558</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C10" s="9" cm="1">
+        <f t="array" aca="1" ref="C10" ca="1">_xll.BDP($B10,C$5,C$4,C$2)</f>
+        <v>1.5773020270736011</v>
+      </c>
+      <c r="D10" s="1">
         <v>4.5444416314450065E-2</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="10" cm="1">
-        <f t="array" aca="1" ref="F10" ca="1">_xll.BDP($B10,F$4,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
+      <c r="E10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="8" cm="1">
+        <f t="array" aca="1" ref="F10" ca="1">_xll.BDP($B10,F$5,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
         <v>33.126138746430001</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="5" t="str" cm="1">
+      <c r="A11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="B11" ca="1">_xll.BDP($B11,B$2)</f>
         <v>TripAdvisor Inc</v>
       </c>
-      <c r="C11" s="1">
-        <v>0.98373997594588491</v>
-      </c>
-      <c r="D11" s="2">
+      <c r="C11" s="9" cm="1">
+        <f t="array" aca="1" ref="C11" ca="1">_xll.BDP($B11,C$5,C$4,C$2)</f>
+        <v>0.85157800625838176</v>
+      </c>
+      <c r="D11" s="1">
         <v>6.8259192108412359E-2</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="10" cm="1">
-        <f t="array" aca="1" ref="F11" ca="1">_xll.BDP($B11,F$4,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
+      <c r="E11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="8" cm="1">
+        <f t="array" aca="1" ref="F11" ca="1">_xll.BDP($B11,F$5,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
         <v>1.9049800625300002</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="6" t="str" cm="1">
+      <c r="A12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="B12" ca="1">_xll.BDP($B12,B$2)</f>
         <v>eBay Inc</v>
       </c>
-      <c r="C12" s="7">
-        <v>2.8940560503324031</v>
-      </c>
-      <c r="D12" s="8">
+      <c r="C12" s="9" cm="1">
+        <f t="array" aca="1" ref="C12" ca="1">_xll.BDP($B12,C$5,C$4,C$2)</f>
+        <v>2.6618605922538481</v>
+      </c>
+      <c r="D12" s="6">
         <v>3.5508948362673376E-2</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="10" cm="1">
-        <f t="array" aca="1" ref="F12" ca="1">_xll.BDP($B12,F$4,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
+      <c r="E12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="8" cm="1">
+        <f t="array" aca="1" ref="F12" ca="1">_xll.BDP($B12,F$5,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
         <v>30.392520000000001</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="6" t="str" cm="1">
+      <c r="A13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="B13" ca="1">_xll.BDP($B13,B$2)</f>
         <v>Amazon.com Inc</v>
       </c>
-      <c r="C13" s="7">
-        <v>2.9831931871505093</v>
-      </c>
-      <c r="D13" s="8">
+      <c r="C13" s="9" cm="1">
+        <f t="array" aca="1" ref="C13" ca="1">_xll.BDP($B13,C$5,C$4,C$2)</f>
+        <v>2.4538533683617874</v>
+      </c>
+      <c r="D13" s="6">
         <v>9.9961851886795516E-2</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="10" cm="1">
-        <f t="array" aca="1" ref="F13" ca="1">_xll.BDP($B13,F$4,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
+      <c r="E13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="8" cm="1">
+        <f t="array" aca="1" ref="F13" ca="1">_xll.BDP($B13,F$5,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
         <v>2083.4076133096801</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="6" t="str" cm="1">
+      <c r="A14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="B14" ca="1">_xll.BDP($B14,B$2)</f>
         <v>Alphabet Inc</v>
       </c>
-      <c r="C14" s="7">
-        <v>6.0814917777501343</v>
-      </c>
-      <c r="D14" s="8">
+      <c r="C14" s="9" cm="1">
+        <f t="array" aca="1" ref="C14" ca="1">_xll.BDP($B14,C$5,C$4,C$2)</f>
+        <v>4.8945812206043744</v>
+      </c>
+      <c r="D14" s="6">
         <v>5.4903076514198679E-2</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="10" cm="1">
-        <f t="array" aca="1" ref="F14" ca="1">_xll.BDP($B14,F$4,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
+      <c r="E14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="8" cm="1">
+        <f t="array" aca="1" ref="F14" ca="1">_xll.BDP($B14,F$5,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
         <v>2011.14598</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="6" t="str" cm="1">
+      <c r="A15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="B15" ca="1">_xll.BDP($B15,B$2)</f>
         <v>Meta Platforms Inc</v>
       </c>
-      <c r="C15" s="7">
-        <v>8.1450410675114764</v>
-      </c>
-      <c r="D15" s="8">
-        <v>0.13742899465468672</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="10" cm="1">
-        <f t="array" aca="1" ref="F15" ca="1">_xll.BDP($B15,F$4,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
+      <c r="C15" s="9" cm="1">
+        <f t="array" aca="1" ref="C15" ca="1">_xll.BDP($B15,C$5,C$4,C$2)</f>
+        <v>6.3397796856771906</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0.13742668984336959</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="8" cm="1">
+        <f t="array" aca="1" ref="F15" ca="1">_xll.BDP($B15,F$5,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
         <v>1534.6627534031497</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="6" t="str" cm="1">
+      <c r="A16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="B16" ca="1">_xll.BDP($B16,B$2)</f>
         <v>Netflix Inc</v>
       </c>
-      <c r="C16" s="7">
-        <v>8.647978249538097</v>
-      </c>
-      <c r="D16" s="8">
+      <c r="C16" s="9" cm="1">
+        <f t="array" aca="1" ref="C16" ca="1">_xll.BDP($B16,C$5,C$4,C$2)</f>
+        <v>6.9368766322053119</v>
+      </c>
+      <c r="D16" s="6">
         <v>0.12273298718510439</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="10" cm="1">
-        <f t="array" aca="1" ref="F16" ca="1">_xll.BDP($B16,F$4,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
+      <c r="E16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="8" cm="1">
+        <f t="array" aca="1" ref="F16" ca="1">_xll.BDP($B16,F$5,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
         <v>382.88538021000005</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="6" t="str" cm="1">
+      <c r="A17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="B17" ca="1">_xll.BDP($B17,B$2)</f>
         <v>Uber Technologies Inc</v>
       </c>
-      <c r="C17" s="7">
-        <v>2.9710628295386883</v>
-      </c>
-      <c r="D17" s="8">
+      <c r="C17" s="9" cm="1">
+        <f t="array" aca="1" ref="C17" ca="1">_xll.BDP($B17,C$5,C$4,C$2)</f>
+        <v>2.2333443924794878</v>
+      </c>
+      <c r="D17" s="6">
         <v>0.14539097880978646</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="10" cm="1">
-        <f t="array" aca="1" ref="F17" ca="1">_xll.BDP($B17,F$4,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
+      <c r="E17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="8" cm="1">
+        <f t="array" aca="1" ref="F17" ca="1">_xll.BDP($B17,F$5,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
         <v>147.58847631224998</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="6" t="str" cm="1">
+      <c r="A18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="B18" ca="1">_xll.BDP($B18,B$2)</f>
         <v>Spotify Technology SA</v>
       </c>
-      <c r="C18" s="7">
-        <v>5.2240243650828324</v>
-      </c>
-      <c r="D18" s="8">
-        <v>0.14663239556283036</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="10" cm="1">
-        <f t="array" aca="1" ref="F18" ca="1">_xll.BDP($B18,F$4,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
+      <c r="C18" s="9" cm="1">
+        <f t="array" aca="1" ref="C18" ca="1">_xll.BDP($B18,C$5,C$4,C$2)</f>
+        <v>4.0205829723191417</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0.14664117920629582</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="8" cm="1">
+        <f t="array" aca="1" ref="F18" ca="1">_xll.BDP($B18,F$5,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
         <v>103.64265147706723</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="6" t="str" cm="1">
+      <c r="A19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="B19" ca="1">_xll.BDP($B19,B$2)</f>
         <v>DoorDash Inc</v>
       </c>
-      <c r="C19" s="7">
-        <v>5.8273346874767826</v>
-      </c>
-      <c r="D19" s="8">
+      <c r="C19" s="9" cm="1">
+        <f t="array" aca="1" ref="C19" ca="1">_xll.BDP($B19,C$5,C$4,C$2)</f>
+        <v>4.2399403141916121</v>
+      </c>
+      <c r="D19" s="6">
         <v>0.18482077569209832</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="10" cm="1">
-        <f t="array" aca="1" ref="F19" ca="1">_xll.BDP($B19,F$4,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
+      <c r="E19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="8" cm="1">
+        <f t="array" aca="1" ref="F19" ca="1">_xll.BDP($B19,F$5,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
         <v>75.612488193440015</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="6" t="str" cm="1">
+      <c r="A20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="B20" ca="1">_xll.BDP($B20,B$2)</f>
         <v>Microsoft Corp</v>
       </c>
-      <c r="C20" s="7">
-        <v>9.6196453247394551</v>
-      </c>
-      <c r="D20" s="8">
-        <v>0.1126019699467895</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="10" cm="1">
-        <f t="array" aca="1" ref="F20" ca="1">_xll.BDP($B20,F$4,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
+      <c r="C20" s="9" cm="1">
+        <f t="array" aca="1" ref="C20" ca="1">_xll.BDP($B20,C$5,C$4,C$2)</f>
+        <v>7.8438029280896542</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.13728692801126208</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="8" cm="1">
+        <f t="array" aca="1" ref="F20" ca="1">_xll.BDP($B20,F$5,"SCALING_FORMAT=BLN","EQY_FUND_CRNCY=USD")</f>
         <v>2828.2585413057491</v>
       </c>
     </row>

</xml_diff>